<commit_message>
Created class to extract Rally data from XLSX file.
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rally\poi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\rally_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Formatted ID</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>As a user, I want to build a dress/closet, to be hipster and store my cloth.</t>
+  </si>
+  <si>
+    <t>Act</t>
   </si>
 </sst>
 </file>
@@ -969,6 +972,9 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -994,6 +1000,9 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1005,6 +1014,9 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1016,6 +1028,9 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1027,6 +1042,9 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1037,6 +1055,9 @@
       </c>
       <c r="C8" t="s">
         <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>